<commit_message>
ajustes en prestamos y convenios
</commit_message>
<xml_diff>
--- a/storage/exports/Prestamos.xlsx
+++ b/storage/exports/Prestamos.xlsx
@@ -10,7 +10,10 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Prestamos" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reporte_Pivot" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Prestamos'!$A$1:$U$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Reporte_Pivot'!$A$1:$L$2</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,13 +430,29 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="14" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="23" customWidth="1" min="19" max="19"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -472,60 +492,70 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>grati jul 25</t>
+          <t>ago 25</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>jul 25</t>
+          <t>set 25</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>ago 25</t>
+          <t>oct 25</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>set 25</t>
+          <t>nov 25</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>oct 25</t>
+          <t>grati dic 25</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>nov 25</t>
+          <t>dic 25</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>grati dic 25</t>
+          <t>ene 26</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>dic 25</t>
+          <t>feb 26</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>ene 26</t>
+          <t>mar 26</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>abr 26</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>may 26</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>MONTO DE AMORTIZACIÓN</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>FECHA DE AMORTIZACIÓN</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>OBS DE AMORTIZACIÓN</t>
         </is>
@@ -550,49 +580,55 @@
           <t>Salud</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>539</v>
+      <c r="E2" s="2" t="n">
+        <v>500</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-07-21</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="G2" t="n">
         <v>2025</v>
       </c>
-      <c r="H2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="I2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="J2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="K2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="L2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="M2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="N2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="O2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="P2" t="n">
-        <v>59.88</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -600,64 +636,692 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>75548700</t>
+          <t>72172994</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CAMILA ESTEFANIA DELGADO YENGLE</t>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Estudios</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>2500</v>
+          <t>Pérdida de Equipos y/o implementos</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>405</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-07-21</t>
+          <t>2025-07-16</t>
         </is>
       </c>
       <c r="G3" t="n">
         <v>2025</v>
       </c>
-      <c r="H3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="I3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="J3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="K3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="L3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="M3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="N3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="O3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>72172994</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Salud</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>405</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="S4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>72172994</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Campaña Compra de Productos</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>405</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="S5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>72172994</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Fallecimiento</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>405</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q6" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="S6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>72172994</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Daño a la infraestructura</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>405</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="R7" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="S7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>72172994</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Catástrofe</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>405</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="R8" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="S8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>72172994</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Estudios hijo</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>405</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="R9" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="S9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>72172994</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Campaña Compra de Productos</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>405</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="R10" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="S10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>72172994</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Salud</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>1250</v>
+      </c>
+      <c r="Q11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>72172994</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ALVARO RODRIGO HERNANDEZ LAOS</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Salud</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="P12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U12"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -668,13 +1332,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="14" customWidth="1" min="11" max="11"/>
+    <col width="17" customWidth="1" min="12" max="12"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -684,45 +1362,55 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Abril 2026</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Agosto 2025</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Diciembre 2025</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Enero 2026</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Febrero 2026</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Gratificación diciembre 2025</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Gratificación julio 2025</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Julio 2025</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Marzo 2026</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Mayo 2026</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Noviembre 2025</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Octubre 2025</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Septiembre 2025</t>
         </is>
@@ -734,69 +1422,42 @@
           <t>72172994</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="C2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="D2" t="n">
-        <v>59.88</v>
-      </c>
-      <c r="E2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="F2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="G2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="H2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="I2" t="n">
-        <v>59.89</v>
-      </c>
-      <c r="J2" t="n">
-        <v>59.89</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>75548700</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="F3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="G3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="H3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="I3" t="n">
-        <v>312.5</v>
-      </c>
-      <c r="J3" t="n">
-        <v>312.5</v>
+      <c r="B2" s="2" t="n">
+        <v>360</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1275</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1697.5</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>1697.5</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>1697.5</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>447.5</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>1672.5</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>360</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1697.5</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>1697.5</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>1337.5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>